<commit_message>
Adding Run mode, Parameterization and Jenkins integrating
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -9,17 +9,37 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9288"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6048"/>
   </bookViews>
   <sheets>
-    <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
+    <sheet name="test_suite" sheetId="1" r:id="rId1"/>
+    <sheet name="AddCustomerTest" sheetId="2" r:id="rId2"/>
+    <sheet name="OpenAccountTest" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
+  <si>
+    <t>TCID</t>
+  </si>
+  <si>
+    <t>Run Mode</t>
+  </si>
+  <si>
+    <t>BankManagerLoginTest</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>AddCustomerTest</t>
+  </si>
+  <si>
+    <t>OpenAccountTest</t>
+  </si>
   <si>
     <t>First Name</t>
   </si>
@@ -30,6 +50,9 @@
     <t>Post Code</t>
   </si>
   <si>
+    <t>Alert Text</t>
+  </si>
+  <si>
     <t>Abdullah</t>
   </si>
   <si>
@@ -39,17 +62,50 @@
     <t>1as123</t>
   </si>
   <si>
-    <t>Alert Text</t>
-  </si>
-  <si>
     <t>Customer added successfully</t>
+  </si>
+  <si>
+    <t>Mohamed</t>
+  </si>
+  <si>
+    <t>1as124</t>
+  </si>
+  <si>
+    <t>Ali</t>
+  </si>
+  <si>
+    <t>1as125</t>
+  </si>
+  <si>
+    <t>Hassan</t>
+  </si>
+  <si>
+    <t>1as126</t>
+  </si>
+  <si>
+    <t>Pound</t>
+  </si>
+  <si>
+    <t>Account created successfully</t>
+  </si>
+  <si>
+    <t>Abdullah Abdel Menem</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>Currency</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -61,6 +117,11 @@
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -83,9 +144,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -304,10 +372,60 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -315,32 +433,129 @@
     <col min="4" max="4" width="25.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
+        <v>20</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>